<commit_message>
changed default latency to 30 in the spreadsheet
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="960" yWindow="0" windowWidth="15180" windowHeight="4830" activeTab="9"/>
+    <workbookView xWindow="1920" yWindow="0" windowWidth="15180" windowHeight="4836" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="exp_1" sheetId="1" r:id="rId1"/>
@@ -419,15 +419,15 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -450,12 +450,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -483,12 +483,12 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -520,12 +520,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>11</v>
       </c>
       <c r="C2">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D2">
         <v>10</v>
@@ -540,12 +540,12 @@
         <v>256</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D3">
         <v>10</v>
@@ -561,12 +561,12 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -578,16 +578,16 @@
         <v>32</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G17" si="0">G3/2</f>
+        <f t="shared" ref="G4:G10" si="0">G3/2</f>
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D5">
         <v>10</v>
@@ -603,12 +603,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D6">
         <v>10</v>
@@ -624,12 +624,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D7">
         <v>10</v>
@@ -645,12 +645,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D8">
         <v>10</v>
@@ -666,12 +666,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>11</v>
       </c>
       <c r="C9">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D9">
         <v>10</v>
@@ -687,12 +687,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D10">
         <v>10</v>
@@ -718,12 +718,12 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D2"/>
+      <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -749,9 +749,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B2">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -763,9 +763,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -777,9 +777,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B4">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -791,9 +791,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B5">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C5">
         <v>10</v>
@@ -815,12 +815,12 @@
   <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="A1:I43"/>
+      <selection activeCell="C2" sqref="C2:C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -849,12 +849,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D2">
         <v>10</v>
@@ -866,12 +866,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D3">
         <v>10</v>
@@ -884,12 +884,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -898,16 +898,16 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F31" si="0">F3*2</f>
+        <f t="shared" ref="F4:F22" si="0">F3*2</f>
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D5">
         <v>10</v>
@@ -920,12 +920,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D6">
         <v>10</v>
@@ -938,12 +938,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D7">
         <v>10</v>
@@ -956,12 +956,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D8">
         <v>10</v>
@@ -974,12 +974,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D9">
         <v>10</v>
@@ -992,12 +992,12 @@
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D10">
         <v>10</v>
@@ -1010,12 +1010,12 @@
         <v>256</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -1028,12 +1028,12 @@
         <v>512</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>10</v>
       </c>
       <c r="C12">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D12">
         <v>10</v>
@@ -1046,12 +1046,12 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>10</v>
       </c>
       <c r="C13">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D13">
         <v>10</v>
@@ -1064,12 +1064,12 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>10</v>
       </c>
       <c r="C14">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D14">
         <v>10</v>
@@ -1082,12 +1082,12 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>10</v>
       </c>
       <c r="C15">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D15">
         <v>10</v>
@@ -1100,12 +1100,12 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>10</v>
       </c>
       <c r="C16">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D16">
         <v>10</v>
@@ -1118,12 +1118,12 @@
         <v>16384</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>10</v>
       </c>
       <c r="C17">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D17">
         <v>10</v>
@@ -1136,12 +1136,12 @@
         <v>32768</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>10</v>
       </c>
       <c r="C18">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D18">
         <v>10</v>
@@ -1154,12 +1154,12 @@
         <v>65536</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>10</v>
       </c>
       <c r="C19">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D19">
         <v>10</v>
@@ -1172,12 +1172,12 @@
         <v>131072</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>10</v>
       </c>
       <c r="C20">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D20">
         <v>10</v>
@@ -1190,12 +1190,12 @@
         <v>262144</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>10</v>
       </c>
       <c r="C21">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D21">
         <v>10</v>
@@ -1208,12 +1208,12 @@
         <v>524288</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>10</v>
       </c>
       <c r="C22">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D22">
         <v>10</v>
@@ -1226,12 +1226,12 @@
         <v>1048576</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>11</v>
       </c>
       <c r="C23">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D23">
         <v>10</v>
@@ -1243,12 +1243,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>11</v>
       </c>
       <c r="C24">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D24">
         <v>10</v>
@@ -1261,12 +1261,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>11</v>
       </c>
       <c r="C25">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D25">
         <v>10</v>
@@ -1279,12 +1279,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>11</v>
       </c>
       <c r="C26">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D26">
         <v>10</v>
@@ -1297,12 +1297,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>11</v>
       </c>
       <c r="C27">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D27">
         <v>10</v>
@@ -1315,12 +1315,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>11</v>
       </c>
       <c r="C28">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D28">
         <v>10</v>
@@ -1333,12 +1333,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>11</v>
       </c>
       <c r="C29">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D29">
         <v>10</v>
@@ -1351,12 +1351,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>11</v>
       </c>
       <c r="C30">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D30">
         <v>10</v>
@@ -1369,12 +1369,12 @@
         <v>128</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>11</v>
       </c>
       <c r="C31">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D31">
         <v>10</v>
@@ -1387,12 +1387,12 @@
         <v>256</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>11</v>
       </c>
       <c r="C32">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D32">
         <v>10</v>
@@ -1405,12 +1405,12 @@
         <v>512</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>11</v>
       </c>
       <c r="C33">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D33">
         <v>10</v>
@@ -1423,12 +1423,12 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>11</v>
       </c>
       <c r="C34">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D34">
         <v>10</v>
@@ -1441,12 +1441,12 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>11</v>
       </c>
       <c r="C35">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D35">
         <v>10</v>
@@ -1459,12 +1459,12 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>11</v>
       </c>
       <c r="C36">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D36">
         <v>10</v>
@@ -1477,12 +1477,12 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>11</v>
       </c>
       <c r="C37">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D37">
         <v>10</v>
@@ -1495,12 +1495,12 @@
         <v>16384</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>11</v>
       </c>
       <c r="C38">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D38">
         <v>10</v>
@@ -1513,12 +1513,12 @@
         <v>32768</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>11</v>
       </c>
       <c r="C39">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D39">
         <v>10</v>
@@ -1531,12 +1531,12 @@
         <v>65536</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>11</v>
       </c>
       <c r="C40">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D40">
         <v>10</v>
@@ -1549,12 +1549,12 @@
         <v>131072</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>11</v>
       </c>
       <c r="C41">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D41">
         <v>10</v>
@@ -1567,12 +1567,12 @@
         <v>262144</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>11</v>
       </c>
       <c r="C42">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D42">
         <v>10</v>
@@ -1585,12 +1585,12 @@
         <v>524288</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>11</v>
       </c>
       <c r="C43">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D43">
         <v>10</v>
@@ -1613,12 +1613,12 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F5"/>
+      <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1650,12 +1650,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>12</v>
       </c>
       <c r="C2">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D2">
         <v>10</v>
@@ -1670,12 +1670,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>12</v>
       </c>
       <c r="C3">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D3">
         <v>10</v>
@@ -1690,12 +1690,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>12</v>
       </c>
       <c r="C4">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -1710,12 +1710,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>12</v>
       </c>
       <c r="C5">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D5">
         <v>10</v>
@@ -1740,12 +1740,12 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F23"/>
+      <selection activeCell="C2" sqref="C2:C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1774,12 +1774,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D2">
         <v>10</v>
@@ -1791,12 +1791,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D3">
         <v>10</v>
@@ -1809,30 +1809,30 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D4">
         <v>10</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E22" si="0">E3+0.2</f>
+        <f t="shared" ref="E4:E12" si="0">E3+0.2</f>
         <v>0.4</v>
       </c>
       <c r="F4">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D5">
         <v>10</v>
@@ -1845,12 +1845,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D6">
         <v>10</v>
@@ -1863,12 +1863,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D7">
         <v>10</v>
@@ -1881,12 +1881,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D8">
         <v>10</v>
@@ -1899,12 +1899,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D9">
         <v>10</v>
@@ -1917,12 +1917,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D10">
         <v>10</v>
@@ -1935,12 +1935,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -1953,12 +1953,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>10</v>
       </c>
       <c r="C12">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D12">
         <v>10</v>
@@ -1971,12 +1971,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D13">
         <v>10</v>
@@ -1988,12 +1988,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="C14">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D14">
         <v>10</v>
@@ -2006,12 +2006,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>11</v>
       </c>
       <c r="C15">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D15">
         <v>10</v>
@@ -2024,12 +2024,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>11</v>
       </c>
       <c r="C16">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D16">
         <v>10</v>
@@ -2042,12 +2042,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>11</v>
       </c>
       <c r="C17">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D17">
         <v>10</v>
@@ -2060,12 +2060,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>11</v>
       </c>
       <c r="C18">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D18">
         <v>10</v>
@@ -2078,12 +2078,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>11</v>
       </c>
       <c r="C19">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D19">
         <v>10</v>
@@ -2096,12 +2096,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>11</v>
       </c>
       <c r="C20">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D20">
         <v>10</v>
@@ -2114,12 +2114,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>11</v>
       </c>
       <c r="C21">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D21">
         <v>10</v>
@@ -2132,12 +2132,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>11</v>
       </c>
       <c r="C22">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D22">
         <v>10</v>
@@ -2150,12 +2150,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>11</v>
       </c>
       <c r="C23">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D23">
         <v>10</v>
@@ -2178,12 +2178,12 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F12"/>
+      <selection activeCell="C2" sqref="C2:C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2215,12 +2215,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>12</v>
       </c>
       <c r="C2">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D2">
         <v>10</v>
@@ -2235,18 +2235,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>12</v>
       </c>
       <c r="C3">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D3">
         <v>10</v>
       </c>
       <c r="E3">
-        <f>E2+0.2</f>
+        <f t="shared" ref="E3:E12" si="0">E2+0.2</f>
         <v>0.2</v>
       </c>
       <c r="F3">
@@ -2256,18 +2256,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>12</v>
       </c>
       <c r="C4">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D4">
         <v>10</v>
       </c>
       <c r="E4">
-        <f>E3+0.2</f>
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
       <c r="F4">
@@ -2277,18 +2277,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>12</v>
       </c>
       <c r="C5">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D5">
         <v>10</v>
       </c>
       <c r="E5">
-        <f>E4+0.2</f>
+        <f t="shared" si="0"/>
         <v>0.60000000000000009</v>
       </c>
       <c r="F5">
@@ -2298,18 +2298,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D6">
         <v>10</v>
       </c>
       <c r="E6">
-        <f>E5+0.2</f>
+        <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
       <c r="F6">
@@ -2319,18 +2319,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D7">
         <v>10</v>
       </c>
       <c r="E7">
-        <f>E6+0.2</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F7">
@@ -2340,18 +2340,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D8">
         <v>10</v>
       </c>
       <c r="E8">
-        <f>E7+0.2</f>
+        <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
       <c r="F8">
@@ -2361,18 +2361,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>12</v>
       </c>
       <c r="C9">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D9">
         <v>10</v>
       </c>
       <c r="E9">
-        <f>E8+0.2</f>
+        <f t="shared" si="0"/>
         <v>1.4</v>
       </c>
       <c r="F9">
@@ -2382,18 +2382,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>12</v>
       </c>
       <c r="C10">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D10">
         <v>10</v>
       </c>
       <c r="E10">
-        <f>E9+0.2</f>
+        <f t="shared" si="0"/>
         <v>1.5999999999999999</v>
       </c>
       <c r="F10">
@@ -2403,18 +2403,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>12</v>
       </c>
       <c r="C11">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D11">
         <v>10</v>
       </c>
       <c r="E11">
-        <f>E10+0.2</f>
+        <f t="shared" si="0"/>
         <v>1.7999999999999998</v>
       </c>
       <c r="F11">
@@ -2424,18 +2424,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="C12">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D12">
         <v>10</v>
       </c>
       <c r="E12">
-        <f>E11+0.2</f>
+        <f t="shared" si="0"/>
         <v>1.9999999999999998</v>
       </c>
       <c r="F12">
@@ -2455,12 +2455,12 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F23"/>
+      <selection activeCell="C2" sqref="C2:C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2489,12 +2489,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D2">
         <v>10</v>
@@ -2506,12 +2506,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D3">
         <v>10</v>
@@ -2524,30 +2524,30 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D4">
         <v>10</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E22" si="0">E3+0.2</f>
+        <f t="shared" ref="E4:E12" si="0">E3+0.2</f>
         <v>0.4</v>
       </c>
       <c r="F4">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D5">
         <v>10</v>
@@ -2560,12 +2560,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D6">
         <v>10</v>
@@ -2578,12 +2578,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D7">
         <v>10</v>
@@ -2596,12 +2596,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D8">
         <v>10</v>
@@ -2614,12 +2614,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D9">
         <v>10</v>
@@ -2632,12 +2632,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D10">
         <v>10</v>
@@ -2650,12 +2650,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -2668,12 +2668,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>10</v>
       </c>
       <c r="C12">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D12">
         <v>10</v>
@@ -2686,12 +2686,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D13">
         <v>10</v>
@@ -2703,12 +2703,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="C14">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D14">
         <v>10</v>
@@ -2721,12 +2721,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>11</v>
       </c>
       <c r="C15">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D15">
         <v>10</v>
@@ -2739,12 +2739,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>11</v>
       </c>
       <c r="C16">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D16">
         <v>10</v>
@@ -2757,12 +2757,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>11</v>
       </c>
       <c r="C17">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D17">
         <v>10</v>
@@ -2775,12 +2775,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>11</v>
       </c>
       <c r="C18">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D18">
         <v>10</v>
@@ -2793,12 +2793,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>11</v>
       </c>
       <c r="C19">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D19">
         <v>10</v>
@@ -2811,12 +2811,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>11</v>
       </c>
       <c r="C20">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D20">
         <v>10</v>
@@ -2829,12 +2829,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>11</v>
       </c>
       <c r="C21">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D21">
         <v>10</v>
@@ -2847,12 +2847,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>11</v>
       </c>
       <c r="C22">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D22">
         <v>10</v>
@@ -2865,12 +2865,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>11</v>
       </c>
       <c r="C23">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D23">
         <v>10</v>
@@ -2893,12 +2893,12 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F12"/>
+      <selection activeCell="C2" sqref="C2:C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2930,12 +2930,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>12</v>
       </c>
       <c r="C2">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D2">
         <v>10</v>
@@ -2950,18 +2950,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>12</v>
       </c>
       <c r="C3">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D3">
         <v>10</v>
       </c>
       <c r="E3">
-        <f>E2+0.2</f>
+        <f t="shared" ref="E3:E12" si="0">E2+0.2</f>
         <v>0.2</v>
       </c>
       <c r="F3">
@@ -2971,18 +2971,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>12</v>
       </c>
       <c r="C4">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D4">
         <v>10</v>
       </c>
       <c r="E4">
-        <f>E3+0.2</f>
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
       <c r="F4">
@@ -2992,18 +2992,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>12</v>
       </c>
       <c r="C5">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D5">
         <v>10</v>
       </c>
       <c r="E5">
-        <f>E4+0.2</f>
+        <f t="shared" si="0"/>
         <v>0.60000000000000009</v>
       </c>
       <c r="F5">
@@ -3013,18 +3013,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D6">
         <v>10</v>
       </c>
       <c r="E6">
-        <f>E5+0.2</f>
+        <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
       <c r="F6">
@@ -3034,18 +3034,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D7">
         <v>10</v>
       </c>
       <c r="E7">
-        <f>E6+0.2</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F7">
@@ -3055,18 +3055,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D8">
         <v>10</v>
       </c>
       <c r="E8">
-        <f>E7+0.2</f>
+        <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
       <c r="F8">
@@ -3076,18 +3076,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>12</v>
       </c>
       <c r="C9">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D9">
         <v>10</v>
       </c>
       <c r="E9">
-        <f>E8+0.2</f>
+        <f t="shared" si="0"/>
         <v>1.4</v>
       </c>
       <c r="F9">
@@ -3097,18 +3097,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>12</v>
       </c>
       <c r="C10">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D10">
         <v>10</v>
       </c>
       <c r="E10">
-        <f>E9+0.2</f>
+        <f t="shared" si="0"/>
         <v>1.5999999999999999</v>
       </c>
       <c r="F10">
@@ -3118,18 +3118,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>12</v>
       </c>
       <c r="C11">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D11">
         <v>10</v>
       </c>
       <c r="E11">
-        <f>E10+0.2</f>
+        <f t="shared" si="0"/>
         <v>1.7999999999999998</v>
       </c>
       <c r="F11">
@@ -3139,18 +3139,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="C12">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D12">
         <v>10</v>
       </c>
       <c r="E12">
-        <f>E11+0.2</f>
+        <f t="shared" si="0"/>
         <v>1.9999999999999998</v>
       </c>
       <c r="F12">
@@ -3170,12 +3170,12 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C2" sqref="C2:C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3198,12 +3198,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D2">
         <v>10</v>
@@ -3215,12 +3215,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D3">
         <v>10</v>
@@ -3233,12 +3233,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -3247,16 +3247,16 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F31" si="0">F3*2</f>
+        <f t="shared" ref="F4:F22" si="0">F3*2</f>
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D5">
         <v>10</v>
@@ -3269,12 +3269,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D6">
         <v>10</v>
@@ -3287,12 +3287,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D7">
         <v>10</v>
@@ -3305,12 +3305,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D8">
         <v>10</v>
@@ -3323,12 +3323,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D9">
         <v>10</v>
@@ -3341,12 +3341,12 @@
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D10">
         <v>10</v>
@@ -3359,12 +3359,12 @@
         <v>256</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -3377,12 +3377,12 @@
         <v>512</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>10</v>
       </c>
       <c r="C12">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D12">
         <v>10</v>
@@ -3395,12 +3395,12 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>10</v>
       </c>
       <c r="C13">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D13">
         <v>10</v>
@@ -3413,12 +3413,12 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>10</v>
       </c>
       <c r="C14">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D14">
         <v>10</v>
@@ -3431,12 +3431,12 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>10</v>
       </c>
       <c r="C15">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D15">
         <v>10</v>
@@ -3449,12 +3449,12 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>10</v>
       </c>
       <c r="C16">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D16">
         <v>10</v>
@@ -3467,12 +3467,12 @@
         <v>16384</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>10</v>
       </c>
       <c r="C17">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D17">
         <v>10</v>
@@ -3485,12 +3485,12 @@
         <v>32768</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>10</v>
       </c>
       <c r="C18">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D18">
         <v>10</v>
@@ -3503,12 +3503,12 @@
         <v>65536</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>10</v>
       </c>
       <c r="C19">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D19">
         <v>10</v>
@@ -3521,12 +3521,12 @@
         <v>131072</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>10</v>
       </c>
       <c r="C20">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D20">
         <v>10</v>
@@ -3539,12 +3539,12 @@
         <v>262144</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>10</v>
       </c>
       <c r="C21">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D21">
         <v>10</v>
@@ -3557,12 +3557,12 @@
         <v>524288</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>10</v>
       </c>
       <c r="C22">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D22">
         <v>10</v>

</xml_diff>